<commit_message>
Tarkington Highschool Senior Football Shoot
Pages and Photos from the Tarkington Highschool Senior Photo Shoot on 09/04/2023 - Class of 2024
</commit_message>
<xml_diff>
--- a/pages/rodeo/massImageUploadSpreadsheet.xlsx
+++ b/pages/rodeo/massImageUploadSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samad\Documents\GitHub\SAMProductions_Website\pages\rodeo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1AEB0B0-F767-4C7B-98F6-A0C52AF5EA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6C5F1B-997F-4869-88ED-DF583F4E34A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2141C088-4B83-4772-A220-B5D2C21E34A5}"/>
+    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2141C088-4B83-4772-A220-B5D2C21E34A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="12">
   <si>
     <t>&lt;a href="</t>
   </si>
@@ -62,10 +62,16 @@
     <t>Dayton_CPRA_DK9A7563</t>
   </si>
   <si>
-    <t>23-05-19_SlackAfter_FridayNight/TieDownRoping/DK9A8940</t>
+    <t>TarkingtonHS_DK9A3559</t>
   </si>
   <si>
-    <t>Dayton_CPRA_DK9A8940</t>
+    <t>TarkingtonHS_DK9A4447</t>
+  </si>
+  <si>
+    <t>TarkingtonHS_football_seniorShoot_DayLayton_20/DK9A4447</t>
+  </si>
+  <si>
+    <t>TarkingtonHS_football_seniorShoot_DayLayton_20/DK9A3559</t>
   </si>
 </sst>
 </file>
@@ -461,18 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5228A7-B05A-4B7C-B5E7-09FDDF7C685C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="32.85546875" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
@@ -521,21 +527,662 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="G134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" t="s">
+        <v>10</v>
+      </c>
+      <c r="E135" t="s">
+        <v>4</v>
+      </c>
+      <c r="F135" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G135" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>